<commit_message>
Opção de abrir ou não relatório de pagamentos
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>PixID</t>
   </si>
@@ -43,13 +43,13 @@
     <t>NumProt</t>
   </si>
   <si>
-    <t>Relatório de Pagamentos pix do dia: 22/06/2023 - (Pagos)</t>
-  </si>
-  <si>
-    <t>Raimundo Domingues de Souza</t>
-  </si>
-  <si>
-    <t>isa</t>
+    <t>Relatório de Pagamentos pix do dia: 05/07/2023 - (Todos)</t>
+  </si>
+  <si>
+    <t>Leonardo Falcão Koblitz</t>
+  </si>
+  <si>
+    <t>adm</t>
   </si>
   <si>
     <t>pago</t>
@@ -58,19 +58,10 @@
     <t>bra</t>
   </si>
   <si>
+    <t>Eduardo Rossini Xavier da Silva</t>
+  </si>
+  <si>
     <t>Keyce Felix dos Santos</t>
-  </si>
-  <si>
-    <t>adm</t>
-  </si>
-  <si>
-    <t>John Nigel Wynn</t>
-  </si>
-  <si>
-    <t>con</t>
-  </si>
-  <si>
-    <t>Eduardo Rossini Xavier da Silva</t>
   </si>
   <si>
     <t>Total das taxas de serviço PIX</t>
@@ -194,7 +185,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:I10" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:I9" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="9">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -495,7 +486,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -556,13 +547,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4">
-        <v>134.75</v>
+        <v>150</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
@@ -573,23 +564,19 @@
       <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="3">
-        <v>23</v>
-      </c>
-      <c r="H4" s="3">
-        <v>14052</v>
-      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4">
-        <v>140.58</v>
+        <v>1934.23</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>11</v>
@@ -598,7 +585,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -606,91 +593,56 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4">
-        <v>140.09</v>
+        <v>934.23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3">
-        <v>23</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1420</v>
-      </c>
-      <c r="I6" s="3">
-        <v>541500</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4">
-        <v>1004.23</v>
+        <v>924.0700000000001</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3">
-        <v>544120</v>
-      </c>
+      <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="3">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4">
-        <v>205.4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="3">
-        <v>23</v>
-      </c>
-      <c r="H8" s="3">
-        <v>14582</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4">
-        <v>6.25</v>
+    <row r="9" spans="1:9">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>